<commit_message>
Update Pertanggal 30 Januari 2026 15:22 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Progress - Master Data Insertion.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Progress - Master Data Insertion.xlsx
@@ -529,15 +529,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -545,22 +536,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -616,6 +595,27 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -925,7 +925,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -942,294 +942,294 @@
   <sheetData>
     <row r="1" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="30"/>
+      <c r="F2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="11"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="2:8" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="2:8" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="22">
         <v>632</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="23">
         <v>632</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="24">
         <v>632</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="23">
         <v>632</v>
       </c>
-      <c r="G5" s="21">
-        <f>IF(D5&gt;0, F5/D5, "")</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="22">
-        <f>IF(E5&gt;0, F5/E5, "")</f>
+      <c r="G5" s="14">
+        <f t="shared" ref="G5:G12" si="0">IF(D5&gt;0, F5/D5, "")</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="15">
+        <f t="shared" ref="H5:H14" si="1">IF(E5&gt;0, F5/E5, "")</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="22">
         <v>534</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="25">
         <v>534</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="26">
         <v>534</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="25">
         <v>534</v>
       </c>
-      <c r="G6" s="23">
-        <f>IF(D6&gt;0, F6/D6, "")</f>
-        <v>1</v>
-      </c>
-      <c r="H6" s="24">
-        <f>IF(E6&gt;0, F6/E6, "")</f>
+      <c r="G6" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H6" s="17">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="29">
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="22">
         <v>617</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="25">
         <v>617</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="26">
         <v>617</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="25">
         <v>617</v>
       </c>
-      <c r="G7" s="23">
-        <f>IF(D7&gt;0, F7/D7, "")</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="24">
-        <f>IF(E7&gt;0, F7/E7, "")</f>
+      <c r="G7" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="17">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="22">
         <v>75</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="25">
         <v>75</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="26">
         <v>75</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="25">
         <v>75</v>
       </c>
-      <c r="G8" s="23">
-        <f>IF(D8&gt;0, F8/D8, "")</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="24">
-        <f>IF(E8&gt;0, F8/E8, "")</f>
+      <c r="G8" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="17">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="22">
         <v>4169</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="25">
         <v>4169</v>
       </c>
-      <c r="E9" s="33">
-        <v>435</v>
-      </c>
-      <c r="F9" s="32">
-        <v>435</v>
-      </c>
-      <c r="G9" s="23">
-        <f>IF(D9&gt;0, F9/D9, "")</f>
-        <v>0.10434156872151595</v>
-      </c>
-      <c r="H9" s="24">
-        <f>IF(E9&gt;0, F9/E9, "")</f>
+      <c r="E9" s="26">
+        <v>1366</v>
+      </c>
+      <c r="F9" s="25">
+        <v>1366</v>
+      </c>
+      <c r="G9" s="16">
+        <f t="shared" si="0"/>
+        <v>0.3276565123530823</v>
+      </c>
+      <c r="H9" s="17">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="22">
         <v>59</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="25">
         <v>59</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="26">
         <v>59</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="25">
         <v>59</v>
       </c>
-      <c r="G10" s="23">
-        <f>IF(D10&gt;0, F10/D10, "")</f>
-        <v>1</v>
-      </c>
-      <c r="H10" s="24">
-        <f>IF(E10&gt;0, F10/E10, "")</f>
+      <c r="G10" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="17">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="22">
         <v>11627</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="25">
         <f>4528+284</f>
         <v>4812</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="23">
-        <f>IF(D11&gt;0, F11/D11, "")</f>
+      <c r="E11" s="26"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="24" t="str">
-        <f>IF(E11&gt;0, F11/E11, "")</f>
+      <c r="H11" s="17" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="22">
         <v>632</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="25">
         <v>632</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="26">
         <v>632</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="25">
         <v>632</v>
       </c>
-      <c r="G12" s="23">
-        <f>IF(D12&gt;0, F12/D12, "")</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="24">
-        <f>IF(E12&gt;0, F12/E12, "")</f>
+      <c r="G12" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="17">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26" t="str">
-        <f>IF(E13&gt;0, F13/E13, "")</f>
+      <c r="B13" s="5"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35">
+      <c r="B14" s="13"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28">
         <f>SUM(D5:D12)</f>
         <v>11530</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="28">
         <f>SUM(E5:E12)</f>
-        <v>2984</v>
-      </c>
-      <c r="F14" s="35">
+        <v>3915</v>
+      </c>
+      <c r="F14" s="28">
         <f>SUM(F5:F12)</f>
-        <v>2984</v>
-      </c>
-      <c r="G14" s="27">
+        <v>3915</v>
+      </c>
+      <c r="G14" s="20">
         <f>IF(D14&gt;0, F14/D14, "")</f>
-        <v>0.25880312228967911</v>
-      </c>
-      <c r="H14" s="28">
-        <f>IF(E14&gt;0, F14/E14, "")</f>
+        <v>0.33954900260190807</v>
+      </c>
+      <c r="H14" s="21">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Pertanggal 02 Februari 2026 18:47 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Progress - Master Data Insertion.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Progress - Master Data Insertion.xlsx
@@ -925,7 +925,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1111,14 +1111,14 @@
         <v>4169</v>
       </c>
       <c r="E9" s="26">
-        <v>1366</v>
+        <v>1423</v>
       </c>
       <c r="F9" s="25">
-        <v>1366</v>
+        <v>1423</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0.3276565123530823</v>
+        <v>0.3413288558407292</v>
       </c>
       <c r="H9" s="17">
         <f t="shared" si="1"/>
@@ -1161,15 +1161,19 @@
         <f>4528+284</f>
         <v>4812</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="26">
+        <v>4528</v>
+      </c>
+      <c r="F11" s="25">
+        <v>4528</v>
+      </c>
       <c r="G11" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="17" t="str">
+        <v>0.94098088113050704</v>
+      </c>
+      <c r="H11" s="17">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
@@ -1218,15 +1222,15 @@
       </c>
       <c r="E14" s="28">
         <f>SUM(E5:E12)</f>
-        <v>3915</v>
+        <v>8500</v>
       </c>
       <c r="F14" s="28">
         <f>SUM(F5:F12)</f>
-        <v>3915</v>
+        <v>8500</v>
       </c>
       <c r="G14" s="20">
         <f>IF(D14&gt;0, F14/D14, "")</f>
-        <v>0.33954900260190807</v>
+        <v>0.73720728534258462</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Update Pertanggal 3 Februari 2026 19:05 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Progress - Master Data Insertion.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Progress - Master Data Insertion.xlsx
@@ -925,7 +925,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1111,14 +1111,14 @@
         <v>4169</v>
       </c>
       <c r="E9" s="26">
-        <v>1423</v>
+        <v>1520</v>
       </c>
       <c r="F9" s="25">
-        <v>1423</v>
+        <v>1520</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0.3413288558407292</v>
+        <v>0.36459582633725113</v>
       </c>
       <c r="H9" s="17">
         <f t="shared" si="1"/>
@@ -1176,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1222,15 +1222,15 @@
       </c>
       <c r="E14" s="28">
         <f>SUM(E5:E12)</f>
-        <v>8500</v>
+        <v>8597</v>
       </c>
       <c r="F14" s="28">
         <f>SUM(F5:F12)</f>
-        <v>8500</v>
+        <v>8597</v>
       </c>
       <c r="G14" s="20">
         <f>IF(D14&gt;0, F14/D14, "")</f>
-        <v>0.73720728534258462</v>
+        <v>0.74562012142237644</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Update Pertanggal 4 Februari 2026 19:22 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Progress - Master Data Insertion.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Progress - Master Data Insertion.xlsx
@@ -925,7 +925,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1108,17 +1108,18 @@
         <v>4169</v>
       </c>
       <c r="D9" s="25">
-        <v>4169</v>
+        <f>2225+1466</f>
+        <v>3691</v>
       </c>
       <c r="E9" s="26">
-        <v>1520</v>
+        <v>2225</v>
       </c>
       <c r="F9" s="25">
-        <v>1520</v>
+        <v>2225</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0.36459582633725113</v>
+        <v>0.60281766458954211</v>
       </c>
       <c r="H9" s="17">
         <f t="shared" si="1"/>
@@ -1218,19 +1219,19 @@
       <c r="C14" s="27"/>
       <c r="D14" s="28">
         <f>SUM(D5:D12)</f>
-        <v>11530</v>
+        <v>11052</v>
       </c>
       <c r="E14" s="28">
         <f>SUM(E5:E12)</f>
-        <v>8597</v>
+        <v>9302</v>
       </c>
       <c r="F14" s="28">
         <f>SUM(F5:F12)</f>
-        <v>8597</v>
+        <v>9302</v>
       </c>
       <c r="G14" s="20">
         <f>IF(D14&gt;0, F14/D14, "")</f>
-        <v>0.74562012142237644</v>
+        <v>0.84165761853058274</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>

</xml_diff>